<commit_message>
modify the contrace of services
</commit_message>
<xml_diff>
--- a/watchServer/doc/接口契约.xlsx
+++ b/watchServer/doc/接口契约.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -66,15 +66,43 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>LiveCertification</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>long</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>分享直播的ID，开始直播时上传</t>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LiveName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>直播的名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>服务结果：0成功；1失败</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Result</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ErrorMessage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>失败原因描述</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>直播签名，用户服务验证</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LiveId</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -167,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -177,6 +205,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -491,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -511,10 +542,10 @@
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7"/>
+      <c r="C1" s="8"/>
       <c r="D1" s="4" t="s">
         <v>5</v>
       </c>
@@ -523,10 +554,10 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="5">
+      <c r="A2" s="6">
         <v>10000001</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -540,45 +571,71 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="1" t="s">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="E5" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="3"/>
+      <c r="E6" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="3"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
@@ -640,15 +697,21 @@
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27" s="3"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A28" s="3"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A29" s="3"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A2:A7"/>
     <mergeCell ref="B1:C1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
add communication connection business
</commit_message>
<xml_diff>
--- a/watchServer/doc/接口契约.xlsx
+++ b/watchServer/doc/接口契约.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="10000001" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="20000001" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -30,6 +30,82 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Metadata</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LocalMac</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FileSignature</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本机MAC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分享文件签名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LiveName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>直播的名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>服务结果：0成功；1失败</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Result</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ErrorMessage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>失败原因描述</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>直播签名，用户服务验证</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LiveId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CreateLiveRequest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CreateLiveResponse</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>StartLiveRequest</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -38,71 +114,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Metadata</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LocalMac</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FileSignature</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>String</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>String</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>本机MAC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>分享文件签名</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LiveName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>String</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>直播的名称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>服务结果：0成功；1失败</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Result</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ErrorMessage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>失败原因描述</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>直播签名，用户服务验证</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>LiveId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>直播ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本地文件签名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>服务结果：0成功|1服务拒绝|2文件签名不一致</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CommCode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>交互服务号</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -195,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -205,6 +237,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -524,14 +559,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.375" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.5" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.875" style="1" bestFit="1" customWidth="1"/>
@@ -542,99 +577,99 @@
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8"/>
+      <c r="C1" s="9"/>
       <c r="D1" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="6">
+      <c r="A2" s="7">
         <v>10000001</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>3</v>
+      <c r="B2" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="4" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="4" t="s">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
@@ -722,12 +757,127 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A2" s="7">
+        <v>20000001</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>